<commit_message>
Annotated data from initial screen at 50uM and 25uM
</commit_message>
<xml_diff>
--- a/7-2-17_top_7_compound_19_analogues_50uM_25uM t=22.xlsx
+++ b/7-2-17_top_7_compound_19_analogues_50uM_25uM t=22.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elinor\Documents\LtaS-inhibitor-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>User: Xavier</t>
   </si>
@@ -79,13 +79,113 @@
   </si>
   <si>
     <t>% Inhibition</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Negative values arbitrarily set to zero</t>
+  </si>
+  <si>
+    <r>
+      <t>OD</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (t=22) - OD</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (t=0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(Control OD</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (normalised) - OD</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (normalised))/control OD600 (normalised) * 100</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +195,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -573,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:M55"/>
+  <dimension ref="A3:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="S53" sqref="S53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,7 +1431,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>15</v>
       </c>
@@ -1364,12 +1472,12 @@
         <v>0.253</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>1</v>
       </c>
@@ -1407,14 +1515,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3">
-        <f t="shared" ref="C37:M37" si="0">D15-D26</f>
+        <f t="shared" ref="D37:K37" si="0">D15-D26</f>
         <v>1.0559999999999998</v>
       </c>
       <c r="E37" s="3">
@@ -1447,15 +1555,18 @@
       </c>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3">
-        <f t="shared" ref="B38:M38" si="1">D16-D27</f>
+        <f t="shared" ref="D38:K38" si="1">D16-D27</f>
         <v>1.347</v>
       </c>
       <c r="E38" s="3">
@@ -1487,15 +1598,18 @@
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3">
-        <f t="shared" ref="B39:M39" si="2">D17-D28</f>
+        <f t="shared" ref="D39:K39" si="2">D17-D28</f>
         <v>0.91299999999999992</v>
       </c>
       <c r="E39" s="3">
@@ -1528,14 +1642,14 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3">
-        <f t="shared" ref="B40:M40" si="3">D18-D29</f>
+        <f t="shared" ref="D40:K40" si="3">D18-D29</f>
         <v>0.318</v>
       </c>
       <c r="E40" s="3">
@@ -1568,14 +1682,14 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3">
-        <f t="shared" ref="B41:M41" si="4">D19-D30</f>
+        <f t="shared" ref="D41:K41" si="4">D19-D30</f>
         <v>1.4939999999999998</v>
       </c>
       <c r="E41" s="3">
@@ -1609,14 +1723,14 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3">
-        <f t="shared" ref="B42:M42" si="5">D20-D31</f>
+        <f t="shared" ref="D42:K42" si="5">D20-D31</f>
         <v>1.304</v>
       </c>
       <c r="E42" s="3">
@@ -1650,14 +1764,14 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3">
-        <f t="shared" ref="B43:M43" si="6">D21-D32</f>
+        <f t="shared" ref="D43:K43" si="6">D21-D32</f>
         <v>1.5899999999999999</v>
       </c>
       <c r="E43" s="3">
@@ -1691,14 +1805,14 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3">
-        <f t="shared" ref="B44:M44" si="7">D22-D33</f>
+        <f t="shared" ref="D44:K44" si="7">D22-D33</f>
         <v>1.3740000000000001</v>
       </c>
       <c r="E44" s="3">
@@ -1732,50 +1846,38 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <v>2</v>
-      </c>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D47">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E47">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F47">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G47">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H47">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I47">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="J47">
-        <v>9</v>
-      </c>
-      <c r="K47">
-        <v>10</v>
-      </c>
-      <c r="L47">
-        <v>11</v>
-      </c>
-      <c r="M47">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="K47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1810,8 +1912,11 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1846,8 +1951,11 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -1883,7 +1991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -1919,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -1956,7 +2064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -1992,7 +2100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -2029,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Redid and annotated missing analyses for antibacterial assays
</commit_message>
<xml_diff>
--- a/7-2-17_top_7_compound_19_analogues_50uM_25uM t=22.xlsx
+++ b/7-2-17_top_7_compound_19_analogues_50uM_25uM t=22.xlsx
@@ -177,7 +177,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (normalised))/control OD600 (normalised) * 100</t>
+      <t xml:space="preserve"> (normalised))/control OD</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (normalised) * 100</t>
     </r>
   </si>
 </sst>
@@ -684,7 +705,7 @@
   <dimension ref="A3:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="S53" sqref="S53"/>
+      <selection activeCell="R53" sqref="R53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>